<commit_message>
Good checkpoint reading in osm values
</commit_message>
<xml_diff>
--- a/RECI_Compliance Parameter Requirements.xlsx
+++ b/RECI_Compliance Parameter Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AntonSzilasi\Documents\OpenStudio20RPD20Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC610B1A-2561-4681-B699-0B4A228C16AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E70F9D90-34B8-48AF-9B2A-8CE403CE1AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22044" windowHeight="13176" xr2:uid="{CDA76BB6-2554-4DD9-8B93-99B2E5875406}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CDA76BB6-2554-4DD9-8B93-99B2E5875406}"/>
   </bookViews>
   <sheets>
     <sheet name="Comp Param Priority" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'E+ Data Element Status'!$A$1:$P$936</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3151" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3170" uniqueCount="540">
   <si>
     <t>=============</t>
   </si>
@@ -1647,9 +1648,6 @@
     <t>Do</t>
   </si>
   <si>
-    <t>HeatingVentilatingAirConditioningSystem.FanSystem</t>
-  </si>
-  <si>
     <t>Required</t>
   </si>
   <si>
@@ -1672,6 +1670,12 @@
   </si>
   <si>
     <t>ParentId</t>
+  </si>
+  <si>
+    <t>Zone.Surface</t>
+  </si>
+  <si>
+    <t>space</t>
   </si>
 </sst>
 </file>
@@ -1702,7 +1706,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1721,6 +1725,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1734,7 +1750,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1742,6 +1758,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2093,14 +2111,14 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="38.44140625" customWidth="1"/>
     <col min="2" max="2" width="65.33203125" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.21875" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" customWidth="1"/>
     <col min="5" max="5" width="21.5546875" customWidth="1"/>
     <col min="6" max="6" width="50.5546875" bestFit="1" customWidth="1"/>
@@ -2111,34 +2129,34 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>531</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>531</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>532</v>
       </c>
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="E2" t="s">
         <v>537</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>536</v>
       </c>
-      <c r="E2" t="s">
-        <v>538</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>537</v>
-      </c>
       <c r="G2" s="3" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2185,10 +2203,13 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="A6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>71</v>
       </c>
       <c r="F6" t="s">
@@ -2199,10 +2220,13 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="A7" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="8" t="s">
         <v>75</v>
       </c>
       <c r="F7" t="s">
@@ -2213,10 +2237,13 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+      <c r="A8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>74</v>
       </c>
       <c r="F8" t="s">
@@ -2227,10 +2254,13 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+      <c r="A9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="7" t="s">
         <v>76</v>
       </c>
       <c r="F9" t="s">
@@ -2297,8 +2327,11 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>257</v>
+      </c>
       <c r="B14" t="s">
-        <v>530</v>
+        <v>286</v>
       </c>
       <c r="C14" t="s">
         <v>307</v>
@@ -2325,10 +2358,13 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="6" t="s">
+      <c r="A16" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="7" t="s">
         <v>125</v>
       </c>
       <c r="F16" t="s">
@@ -2338,13 +2374,19 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>78</v>
+      </c>
       <c r="B17" t="s">
         <v>337</v>
       </c>
       <c r="C17" t="s">
         <v>353</v>
       </c>
+      <c r="E17" t="s">
+        <v>78</v>
+      </c>
       <c r="F17" t="s">
         <v>105</v>
       </c>
@@ -2352,7 +2394,10 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>78</v>
+      </c>
       <c r="B18" t="s">
         <v>105</v>
       </c>
@@ -2360,6 +2405,9 @@
         <v>113</v>
       </c>
       <c r="D18" s="4"/>
+      <c r="E18" t="s">
+        <v>78</v>
+      </c>
       <c r="F18" t="s">
         <v>105</v>
       </c>
@@ -2367,14 +2415,20 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>78</v>
+      </c>
       <c r="B19" t="s">
-        <v>105</v>
+        <v>539</v>
       </c>
       <c r="C19" t="s">
         <v>116</v>
       </c>
       <c r="D19" s="4"/>
+      <c r="E19" t="s">
+        <v>78</v>
+      </c>
       <c r="F19" t="s">
         <v>105</v>
       </c>
@@ -2382,7 +2436,10 @@
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>78</v>
+      </c>
       <c r="B20" t="s">
         <v>189</v>
       </c>
@@ -2390,6 +2447,9 @@
         <v>193</v>
       </c>
       <c r="D20" s="4"/>
+      <c r="E20" t="s">
+        <v>78</v>
+      </c>
       <c r="F20" t="s">
         <v>189</v>
       </c>
@@ -2397,7 +2457,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>198</v>
       </c>
@@ -2405,6 +2465,9 @@
         <v>36</v>
       </c>
       <c r="D21" s="4"/>
+      <c r="E21" t="s">
+        <v>78</v>
+      </c>
       <c r="F21" t="s">
         <v>130</v>
       </c>
@@ -2412,13 +2475,16 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>198</v>
       </c>
       <c r="C22" t="s">
         <v>205</v>
       </c>
+      <c r="E22" t="s">
+        <v>78</v>
+      </c>
       <c r="F22" t="s">
         <v>169</v>
       </c>
@@ -2426,13 +2492,19 @@
         <v>171</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>538</v>
+      </c>
       <c r="B23" t="s">
         <v>169</v>
       </c>
       <c r="C23" t="s">
         <v>170</v>
       </c>
+      <c r="E23" t="s">
+        <v>78</v>
+      </c>
       <c r="F23" t="s">
         <v>169</v>
       </c>
@@ -2440,7 +2512,10 @@
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>78</v>
+      </c>
       <c r="B24" t="s">
         <v>169</v>
       </c>
@@ -2454,7 +2529,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D25" s="4"/>
       <c r="F25" t="s">
         <v>169</v>
@@ -2463,9 +2538,9 @@
         <v>172</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F26" t="s">
         <v>141</v>
@@ -2474,7 +2549,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
         <v>437</v>
       </c>
@@ -2483,7 +2558,7 @@
       </c>
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
         <v>423</v>
       </c>
@@ -2492,7 +2567,7 @@
       </c>
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
         <v>313</v>
       </c>
@@ -2500,15 +2575,15 @@
         <v>314</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D31" s="4"/>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.3">
@@ -14082,6 +14157,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="141d59ff-0f67-4f50-8344-64b15536f9a6" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2b95255b-60dc-4683-a12c-6b4df4508597">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002623BFAE8B0C414481CE00A23BDDDF22" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5757300bcb8c7282e444b5e121d16c6e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="141d59ff-0f67-4f50-8344-64b15536f9a6" xmlns:ns3="2b95255b-60dc-4683-a12c-6b4df4508597" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3dd4915a0a1810b23a552d1776a3d509" ns2:_="" ns3:_="">
     <xsd:import namespace="141d59ff-0f67-4f50-8344-64b15536f9a6"/>
@@ -14336,27 +14431,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BADE3CCD-7C47-418F-9401-F17AC9167B65}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="141d59ff-0f67-4f50-8344-64b15536f9a6"/>
+    <ds:schemaRef ds:uri="2b95255b-60dc-4683-a12c-6b4df4508597"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="141d59ff-0f67-4f50-8344-64b15536f9a6" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2b95255b-60dc-4683-a12c-6b4df4508597">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAF97DB2-429F-48DA-961D-F826F3AE9771}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DFC6FFF-1878-4E76-9760-53357013A212}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14373,23 +14467,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAF97DB2-429F-48DA-961D-F826F3AE9771}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BADE3CCD-7C47-418F-9401-F17AC9167B65}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="141d59ff-0f67-4f50-8344-64b15536f9a6"/>
-    <ds:schemaRef ds:uri="2b95255b-60dc-4683-a12c-6b4df4508597"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>